<commit_message>
Straightening Out All the Previously Spaghettified Code
</commit_message>
<xml_diff>
--- a/actuarial-tasks/www/sorp_database_template.xlsx
+++ b/actuarial-tasks/www/sorp_database_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tommycornally/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tommycornally/Documents/Actuarial Tasks in R/actuarial-tasks/www/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8AD2D8-0692-5B4F-B902-5455E715F16A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1D8E0C-3A2D-2449-A410-F575FCBC1851}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15780" xr2:uid="{B6E56F0C-D64D-49B4-B21E-7FC6957AEEA8}"/>
   </bookViews>
@@ -33,6 +33,24 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={921DDDBE-AB9E-CE4F-8266-57C5EAB1EE1D}</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{921DDDBE-AB9E-CE4F-8266-57C5EAB1EE1D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    (Single = 1; Married = 2)</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
@@ -68,15 +86,21 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="&quot;€&quot;#,##0"/>
+    <numFmt numFmtId="164" formatCode="&quot;€&quot;#,##0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,7 +128,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -128,7 +152,9 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Cornally, Tommy" id="{51F6A88F-089F-5F42-8367-D7192D9AF7E9}" userId="S::117378663@umail.ucc.ie::80d491ca-50cc-4d08-9af3-3f77cd6af676" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -426,12 +452,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C1" dT="2021-03-01T14:59:30.71" personId="{51F6A88F-089F-5F42-8367-D7192D9AF7E9}" id="{921DDDBE-AB9E-CE4F-8266-57C5EAB1EE1D}">
+    <text>(Single = 1; Married = 2)</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BE43AA3-DE68-4878-8EDE-057042EC31B2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BE43AA3-DE68-4878-8EDE-057042EC31B2}">
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -534,5 +568,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>